<commit_message>
Add test case: blackbox testcase
</commit_message>
<xml_diff>
--- a/Testcase/blackbox.xlsx
+++ b/Testcase/blackbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buiqu\OneDrive\Documents\GitHub\OnlineShop\Testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345B1837-516E-4CB6-A53C-5ECEE3D53586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE04F5D3-78A4-4365-AB13-97553D16086D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{23446A08-8C0D-4719-9633-89381A1415D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{23446A08-8C0D-4719-9633-89381A1415D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="67">
   <si>
     <t>Input</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Nhập &gt;50 kí tự</t>
   </si>
 </sst>
 </file>
@@ -320,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -671,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51817139-E771-4CE7-A9CF-AD4A694FA1FC}">
   <dimension ref="C1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,10 +707,10 @@
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -712,24 +718,24 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -737,15 +743,15 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
@@ -766,7 +772,7 @@
   <dimension ref="C1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,10 +801,10 @@
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -806,24 +812,24 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -831,24 +837,24 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -856,24 +862,24 @@
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -881,24 +887,24 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -906,24 +912,24 @@
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="1" t="s">
-        <v>7</v>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -931,33 +937,33 @@
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="1" t="s">
-        <v>7</v>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
       <c r="E21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C10:C12"/>
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -967,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3F6B4-71E2-45CC-AA60-BC12D3CCA6D8}">
   <dimension ref="C1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,10 +1003,10 @@
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1008,24 +1014,24 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1033,24 +1039,24 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1058,87 +1064,87 @@
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="10"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="10"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="9"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="7" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1146,17 +1152,17 @@
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1164,35 +1170,41 @@
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="9"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="10"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="E13:E15"/>
@@ -1209,12 +1221,6 @@
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1224,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F2E93C-4657-4755-9C7C-BAFED224BF41}">
   <dimension ref="C1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,10 +1260,10 @@
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1265,24 +1271,24 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1290,60 +1296,60 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="10"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="10"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1396,10 +1402,10 @@
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1407,24 +1413,24 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1432,24 +1438,24 @@
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1457,106 +1463,106 @@
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="10"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="10"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="10"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="8"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
@@ -1570,34 +1576,34 @@
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:E28"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="E21:E22"/>
@@ -1610,12 +1616,12 @@
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update testcase: black, white, unit, testcase, testplan
</commit_message>
<xml_diff>
--- a/Testcase/blackbox.xlsx
+++ b/Testcase/blackbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\buiqu\OneDrive\Documents\GitHub\OnlineShop\Testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE04F5D3-78A4-4365-AB13-97553D16086D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318BD0BF-7EF6-40A1-A595-8F155F5A92CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{23446A08-8C0D-4719-9633-89381A1415D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{23446A08-8C0D-4719-9633-89381A1415D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="66">
   <si>
     <t>Input</t>
   </si>
@@ -43,9 +43,6 @@
     <t>ValidInput</t>
   </si>
   <si>
-    <t>IsvalidInput</t>
-  </si>
-  <si>
     <t>Phân vùng tương đương</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>Nhập &lt;1 kí tự</t>
   </si>
   <si>
-    <t>Nhập &gt;51 kí tự</t>
-  </si>
-  <si>
     <t>Mật khẩu</t>
   </si>
   <si>
@@ -88,15 +82,6 @@
     <t>Nhập chuỗi kí tự email hợp lệ trong khoảng 1 - 50 kí tự</t>
   </si>
   <si>
-    <t>Nhập số điện thoại hợp lệ trong khoảng 9 - 10 số</t>
-  </si>
-  <si>
-    <t>Nhập &lt;9 số</t>
-  </si>
-  <si>
-    <t>Nhập &gt;10 số</t>
-  </si>
-  <si>
     <t>Để trống không nhập gì hoặc nhập kí tự chữ</t>
   </si>
   <si>
@@ -115,9 +100,6 @@
     <t>Nhập &lt;0 kí tự</t>
   </si>
   <si>
-    <t>Nhập &gt;251 kí tự</t>
-  </si>
-  <si>
     <t>Mã sản phẩm</t>
   </si>
   <si>
@@ -145,9 +127,6 @@
     <t>Nhập kí tự trong khoảng 1 - 10 kí tự</t>
   </si>
   <si>
-    <t>Nhập &gt;11 kí tự</t>
-  </si>
-  <si>
     <t>Nhập kí tự trong khoảng 1 - 250 kí tự (tự động nhập khi nhập tên sản phẩm</t>
   </si>
   <si>
@@ -160,9 +139,6 @@
     <t>Nhập kí tự trong khoảng 1 - 500 kí tự</t>
   </si>
   <si>
-    <t>Nhập &gt;501 kí tự</t>
-  </si>
-  <si>
     <t>Nhập số tiền</t>
   </si>
   <si>
@@ -236,6 +212,27 @@
   </si>
   <si>
     <t>Nhập &gt;50 kí tự</t>
+  </si>
+  <si>
+    <t>Nhập &gt;250 kí tự</t>
+  </si>
+  <si>
+    <t>Nhập &gt;500 kí tự</t>
+  </si>
+  <si>
+    <t>Nhập &gt;10 kí tự</t>
+  </si>
+  <si>
+    <t>Nhập số điện thoại hợp lệ trong khoảng 6 - 20 số</t>
+  </si>
+  <si>
+    <t>Nhập &lt;6 số</t>
+  </si>
+  <si>
+    <t>Nhập &gt;20 số</t>
+  </si>
+  <si>
+    <t>InvalidInput</t>
   </si>
 </sst>
 </file>
@@ -678,7 +675,7 @@
   <dimension ref="C1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,7 +689,7 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.3">
@@ -703,57 +700,57 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +769,7 @@
   <dimension ref="C1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +783,7 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.3">
@@ -797,173 +794,173 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -974,7 +971,7 @@
   <dimension ref="C1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C28"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +985,7 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.3">
@@ -999,93 +996,93 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
@@ -1100,13 +1097,13 @@
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
@@ -1121,13 +1118,13 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
@@ -1142,49 +1139,49 @@
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
@@ -1199,12 +1196,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="D26:D28"/>
     <mergeCell ref="E13:E15"/>
@@ -1221,6 +1212,12 @@
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1230,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F2E93C-4657-4755-9C7C-BAFED224BF41}">
   <dimension ref="C1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1245,7 +1242,7 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.3">
@@ -1256,68 +1253,68 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
@@ -1332,13 +1329,13 @@
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
@@ -1372,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518B5A49-EB3C-4D55-B531-823D7B924C67}">
   <dimension ref="C1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,7 +1384,7 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.3">
@@ -1398,93 +1395,93 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="3" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="7" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
@@ -1499,10 +1496,10 @@
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E16" s="9"/>
     </row>
@@ -1518,13 +1515,13 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
@@ -1534,13 +1531,13 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
@@ -1550,13 +1547,13 @@
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
@@ -1566,24 +1563,24 @@
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
@@ -1598,12 +1595,12 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="E21:E22"/>
@@ -1616,12 +1613,12 @@
     <mergeCell ref="E16:E18"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>